<commit_message>
set column type as date
</commit_message>
<xml_diff>
--- a/AD419.DataHelper.Web/Content/Sample_Forms/ProjectsForImport.xlsx
+++ b/AD419.DataHelper.Web/Content/Sample_Forms/ProjectsForImport.xlsx
@@ -365,8 +365,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -649,8 +650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -669,11 +670,11 @@
     <col min="14" max="14" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="16" max="17" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="27.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="15" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="13.28515625" bestFit="1" customWidth="1"/>
@@ -731,10 +732,10 @@
       <c r="Q1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
       <c r="T1" t="s">
@@ -743,7 +744,7 @@
       <c r="U1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="V1" s="1" t="s">
         <v>21</v>
       </c>
       <c r="W1" t="s">
@@ -796,16 +797,16 @@
       <c r="N2" t="s">
         <v>36</v>
       </c>
-      <c r="R2">
+      <c r="R2" s="1">
         <v>40909</v>
       </c>
-      <c r="S2">
+      <c r="S2" s="1">
         <v>41500</v>
       </c>
       <c r="T2">
         <v>2013</v>
       </c>
-      <c r="V2">
+      <c r="V2" s="1">
         <v>41600</v>
       </c>
       <c r="W2" t="s">
@@ -840,10 +841,10 @@
       <c r="K3" t="s">
         <v>44</v>
       </c>
-      <c r="R3">
+      <c r="R3" s="1">
         <v>41183</v>
       </c>
-      <c r="S3">
+      <c r="S3" s="1">
         <v>43008</v>
       </c>
       <c r="T3">
@@ -887,16 +888,16 @@
       <c r="O4">
         <v>100</v>
       </c>
-      <c r="R4">
+      <c r="R4" s="1">
         <v>40817</v>
       </c>
-      <c r="S4">
+      <c r="S4" s="1">
         <v>42004</v>
       </c>
       <c r="T4">
         <v>2013</v>
       </c>
-      <c r="V4">
+      <c r="V4" s="1">
         <v>42039</v>
       </c>
       <c r="W4" t="s">
@@ -931,16 +932,16 @@
       <c r="K5" t="s">
         <v>44</v>
       </c>
-      <c r="R5">
+      <c r="R5" s="1">
         <v>39356</v>
       </c>
-      <c r="S5">
+      <c r="S5" s="1">
         <v>41182</v>
       </c>
       <c r="T5">
         <v>2012</v>
       </c>
-      <c r="V5">
+      <c r="V5" s="1">
         <v>41361</v>
       </c>
       <c r="W5" t="s">
@@ -981,10 +982,10 @@
       <c r="O6">
         <v>100</v>
       </c>
-      <c r="R6">
+      <c r="R6" s="1">
         <v>41936</v>
       </c>
-      <c r="S6">
+      <c r="S6" s="1">
         <v>43738</v>
       </c>
       <c r="W6" t="s">
@@ -1025,10 +1026,10 @@
       <c r="O7">
         <v>100</v>
       </c>
-      <c r="R7">
+      <c r="R7" s="1">
         <v>41922</v>
       </c>
-      <c r="S7">
+      <c r="S7" s="1">
         <v>43738</v>
       </c>
       <c r="W7" t="s">
@@ -1075,10 +1076,10 @@
       <c r="Q8">
         <v>5</v>
       </c>
-      <c r="R8">
+      <c r="R8" s="1">
         <v>42278</v>
       </c>
-      <c r="S8">
+      <c r="S8" s="1">
         <v>44104</v>
       </c>
       <c r="W8" t="s">
@@ -1119,10 +1120,10 @@
       <c r="O9">
         <v>100</v>
       </c>
-      <c r="R9">
+      <c r="R9" s="1">
         <v>41978</v>
       </c>
-      <c r="S9">
+      <c r="S9" s="1">
         <v>43738</v>
       </c>
       <c r="W9" t="s">
@@ -1157,10 +1158,10 @@
       <c r="K10" t="s">
         <v>50</v>
       </c>
-      <c r="R10">
+      <c r="R10" s="1">
         <v>39722</v>
       </c>
-      <c r="S10">
+      <c r="S10" s="1">
         <v>40862</v>
       </c>
       <c r="T10">
@@ -1222,13 +1223,13 @@
       <c r="Q11">
         <v>90</v>
       </c>
-      <c r="R11">
+      <c r="R11" s="1">
         <v>41760</v>
       </c>
-      <c r="S11">
+      <c r="S11" s="1">
         <v>42124</v>
       </c>
-      <c r="V11">
+      <c r="V11" s="1">
         <v>42129</v>
       </c>
       <c r="W11" t="s">
@@ -1287,10 +1288,10 @@
       <c r="Q12">
         <v>10</v>
       </c>
-      <c r="R12">
+      <c r="R12" s="1">
         <v>41518</v>
       </c>
-      <c r="S12">
+      <c r="S12" s="1">
         <v>42613</v>
       </c>
       <c r="T12">
@@ -1305,5 +1306,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>